<commit_message>
upd: finished all testcases
</commit_message>
<xml_diff>
--- a/src/main/resources/FindingHospitalsTestCases.xlsx
+++ b/src/main/resources/FindingHospitalsTestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\projects\eclipse_workspace\FindingHospitals\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8622ABA2-830C-468A-95D7-6A871D8036D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6264954-A79A-4B0A-9B67-BD161AA9E99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="103">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -193,6 +193,200 @@
   </si>
   <si>
     <t>SMOKE</t>
+  </si>
+  <si>
+    <t>TS_2_TC_1</t>
+  </si>
+  <si>
+    <t>Filter for Male Doctors</t>
+  </si>
+  <si>
+    <t>1. Navigate to Practo Homepage
+2. Scroll down and select "Search for doctors" under the "For Patients" sub-section in the footer.</t>
+  </si>
+  <si>
+    <t>1. Select the "Male Doctors" option under the gender dropdown.
+2. Record the number of doctors available and get the top 5 names.</t>
+  </si>
+  <si>
+    <t>1. Select "Male Doctors" option under the gender dropdown.
+2. Select the "20+ Patient Stories" options under the Patient stories dropdown.
+3. Record the number of doctors available and get the top 5 names.</t>
+  </si>
+  <si>
+    <t>Filter Male doctors by
+patient stories</t>
+  </si>
+  <si>
+    <t>Filter Female doctors by
+patient stories</t>
+  </si>
+  <si>
+    <t>Filter by experience</t>
+  </si>
+  <si>
+    <t>1. Filter by 5+ years of experience.
+2. Record the number of doctors available and get the top 5 names.</t>
+  </si>
+  <si>
+    <t>1. Filter by 10+ years of experience.
+2. Record the number of doctors available and get the top 5 names.</t>
+  </si>
+  <si>
+    <t>1. Filter by 15+ years of experience.
+2. Record the number of doctors available and get the top 5 names.</t>
+  </si>
+  <si>
+    <t>1. Filter by 20+ years of experience.
+2. Record the number of doctors available and get the top 5 names.</t>
+  </si>
+  <si>
+    <t>Filter for Female Doctors</t>
+  </si>
+  <si>
+    <t>1. Select the "Female Doctors" option under the gender dropdown.
+2. Record the number of doctors available and get the top 5 names.</t>
+  </si>
+  <si>
+    <t>TS_2_TC_2</t>
+  </si>
+  <si>
+    <t>TS_2_TC_3</t>
+  </si>
+  <si>
+    <t>TS_2_TC_4</t>
+  </si>
+  <si>
+    <t>TS_2_TC_5</t>
+  </si>
+  <si>
+    <t>TS_2_TC_6</t>
+  </si>
+  <si>
+    <t>TS_2_TC_7</t>
+  </si>
+  <si>
+    <t>TS_2_TC_8</t>
+  </si>
+  <si>
+    <t>REGRESSION</t>
+  </si>
+  <si>
+    <t>TS_3_TC_1</t>
+  </si>
+  <si>
+    <t>1. Navigate to Practo Homepage
+2. Scroll down and select "Search for clinics" under the "For Patients" sub-section in the footer.</t>
+  </si>
+  <si>
+    <t>1. Get the names of the first 10 clinics.
+2. Get their rating.
+3. Get timings.
+4. Get location.</t>
+  </si>
+  <si>
+    <t>TS_4_TC_1</t>
+  </si>
+  <si>
+    <t>Get the names of hospitals
+which are open 24/7.</t>
+  </si>
+  <si>
+    <t>1. Navigate to Practo Homepage
+2. Scroll down and select "Search for hospitals" under the "For Patients" sub-section in the footer.</t>
+  </si>
+  <si>
+    <t>1. Check if the timing of the hospital is listed as "MON - SUN 00:00AM - 11:59PM".
+2. If yes, capture the name of the hospital.</t>
+  </si>
+  <si>
+    <t>Get the names of hospitals
+which have a rating higher than 3.5.</t>
+  </si>
+  <si>
+    <t>1. Check if the rating of the hospital is greater than 3.5.
+2. If yes, capture the name of the hospital, rating, and location.</t>
+  </si>
+  <si>
+    <t>TS_4_TC_2</t>
+  </si>
+  <si>
+    <t>TS_5_TC_1</t>
+  </si>
+  <si>
+    <t>Get the list of top cities
+in the pop-up.</t>
+  </si>
+  <si>
+    <t>1. Navigate to Practo Homepage.
+2. Select Lab Tests from the navigation bar.</t>
+  </si>
+  <si>
+    <t>1. Get a list of all the cities listed under top cities.</t>
+  </si>
+  <si>
+    <t>TS_5_TC_2</t>
+  </si>
+  <si>
+    <t>Get the list of all the cities in the pop-up.</t>
+  </si>
+  <si>
+    <t>1. Get all the cities listed and store them.</t>
+  </si>
+  <si>
+    <t>TS_6_TC_1</t>
+  </si>
+  <si>
+    <t>Fill the form with correct
+details.</t>
+  </si>
+  <si>
+    <t>1. Navigate to Practo Homepage.
+2. Select "Health &amp; Wellness Plans" under the "For Corporates" dropdown.</t>
+  </si>
+  <si>
+    <t>1. Give "Sai Nivas" as input in the Name field.
+2. Give "Cognizant" as input in the Organization field.
+3. Give a randomly generated 5 digit number as input in the contact number field.
+4. Give an invalid email ID as input in the Email field.
+5. Select any organization size.
+6. Select any one option in the "Interested in" dropdown.
+7. Check if the "Schedule a demo" button is enabled.</t>
+  </si>
+  <si>
+    <t>Fill the form with incorrect
+details.</t>
+  </si>
+  <si>
+    <t>TS_6_TC_2</t>
+  </si>
+  <si>
+    <t>TS_6_TC_3</t>
+  </si>
+  <si>
+    <t>1. Give "Sai Nivas" as input in the Name field.
+2. Give "Cognizant" as input in the Organization field.
+3. Give a randomly generated 10 digit number as input in the contact number field.
+4. Give a valid email ID as input in the Email field.
+5. Select any organization size.
+6. Select any one option in the "Interested in" dropdown.
+7. Check if the "Schedule a demo" button is enabled.</t>
+  </si>
+  <si>
+    <t>Verify placeholder text.</t>
+  </si>
+  <si>
+    <t>1. The name input field should contain a placeholder
+text "Name".
+2. The organization name input field should contain
+a placeholder text "Organization Name".
+3. The mobile number input field should contain
+a placeholder text "Contact Number".
+4. The email ID input field should contain a
+placeholder text "Official Email ID".</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -234,7 +428,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -257,30 +451,125 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -563,141 +852,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="22" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="G6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -712,19 +1004,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B2F924-59CD-4B6B-A324-085C6D5C9E40}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
@@ -753,93 +1046,345 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="D4" s="20"/>
+      <c r="E4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="D5" s="20"/>
+      <c r="E5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="D6" s="21"/>
+      <c r="E6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="16">
+    <mergeCell ref="F7:F15"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="A20:A22"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="F2:F6"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="A7:A14"/>
+    <mergeCell ref="D7:D14"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>